<commit_message>
Major tweaks included to solve sync issues
</commit_message>
<xml_diff>
--- a/automation.cucumber/src/main/resources/objects.xlsx
+++ b/automation.cucumber/src/main/resources/objects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="24180" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
   <si>
     <t>elementID</t>
   </si>
@@ -258,9 +258,6 @@
     <t>searchButton</t>
   </si>
   <si>
-    <t>//*[@id="center_column"]/ul/li</t>
-  </si>
-  <si>
     <t>searchResults</t>
   </si>
   <si>
@@ -303,15 +300,9 @@
     <t>addToCart</t>
   </si>
   <si>
-    <t>//*[contains(text(), 'Product successfully added to your shopping cart')]</t>
-  </si>
-  <si>
     <t>addtoCart_confirmationMessage</t>
   </si>
   <si>
-    <t>a[title='Proceed to checkout']</t>
-  </si>
-  <si>
     <t>proceedToCheckout</t>
   </si>
   <si>
@@ -321,9 +312,6 @@
     <t>shoppingCartSummary</t>
   </si>
   <si>
-    <t>//*[@id="product_2_8_0_278894"]/td[2]/small[2]</t>
-  </si>
-  <si>
     <t>description_prodSummaryPage</t>
   </si>
   <si>
@@ -336,14 +324,35 @@
     <t>priceOfPerProduct</t>
   </si>
   <si>
-    <t>totalPrice_prodSummaryPage</t>
+    <t>//ul[@class="product_list grid row"]/li</t>
+  </si>
+  <si>
+    <t>//*[@id="layer_cart"]/div[1]/div[1]/h2</t>
+  </si>
+  <si>
+    <t>//a[@title="Proceed to checkout"]</t>
+  </si>
+  <si>
+    <t>//td[@class="cart_description"]/small[2]</t>
+  </si>
+  <si>
+    <t>total_product</t>
+  </si>
+  <si>
+    <t>totalProduct</t>
+  </si>
+  <si>
+    <t>total_shipping</t>
+  </si>
+  <si>
+    <t>total_tax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,12 +366,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="9.8000000000000007"/>
@@ -397,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -406,8 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,17 +692,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1078,7 +1080,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1089,7 +1091,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1111,7 +1113,7 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1122,7 +1124,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1133,162 +1135,195 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>80</v>
+      <c r="A40" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="B46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
         <v>89</v>
-      </c>
-      <c r="C46" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="C47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
-        <v>93</v>
+      <c r="A48" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>95</v>
+      <c r="A49" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C50" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="4" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>101</v>
+      <c r="A52" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" t="s">
-        <v>102</v>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B56">
       <formula1>"ID,ClassName,LinkText,CSS_Selector,TagName,Xpath,Name,PartialLinkText"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added reporting features and completed @addItemstoCart
</commit_message>
<xml_diff>
--- a/automation.cucumber/src/main/resources/objects.xlsx
+++ b/automation.cucumber/src/main/resources/objects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="24180" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="41850" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="114">
   <si>
     <t>elementID</t>
   </si>
@@ -180,18 +180,12 @@
     <t>submitAccount</t>
   </si>
   <si>
-    <t>id_gender1</t>
-  </si>
-  <si>
     <t>reg_salutation_Mr</t>
   </si>
   <si>
     <t>reg_salutation_Mrs</t>
   </si>
   <si>
-    <t>id_gender2</t>
-  </si>
-  <si>
     <t>reg_firstName1</t>
   </si>
   <si>
@@ -213,15 +207,9 @@
     <t>myPersonalInformationMenu</t>
   </si>
   <si>
-    <t>//*[@id="center_column"]/div/div[1]/ul/li[4]</t>
-  </si>
-  <si>
     <t>myPersonalInformationHeading</t>
   </si>
   <si>
-    <t>//*[contains(text(), 'Your personal information')]</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -303,9 +291,6 @@
     <t>addtoCart_confirmationMessage</t>
   </si>
   <si>
-    <t>proceedToCheckout</t>
-  </si>
-  <si>
     <t>//*[contains(text(), 'Shopping-cart summary')]</t>
   </si>
   <si>
@@ -330,9 +315,6 @@
     <t>//*[@id="layer_cart"]/div[1]/div[1]/h2</t>
   </si>
   <si>
-    <t>//a[@title="Proceed to checkout"]</t>
-  </si>
-  <si>
     <t>//td[@class="cart_description"]/small[2]</t>
   </si>
   <si>
@@ -346,6 +328,39 @@
   </si>
   <si>
     <t>total_tax</t>
+  </si>
+  <si>
+    <t>//*[@id="center_column"]/div/div[1]/ul/li[4]/a/span</t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>page-subheading</t>
+  </si>
+  <si>
+    <t>//*[@id="layer_cart"]/div[1]/div[2]/div[4]/a</t>
+  </si>
+  <si>
+    <t>proceedToCheckout_checkOutPage</t>
+  </si>
+  <si>
+    <t>proceedToCheckout_popUp</t>
+  </si>
+  <si>
+    <t>//*[@id="center_column"]/p[2]/a[1]</t>
+  </si>
+  <si>
+    <t>signOutButton</t>
+  </si>
+  <si>
+    <t>//a[contains(@title,'Log me out')]</t>
+  </si>
+  <si>
+    <t>//*[@id="id_gender1"]</t>
+  </si>
+  <si>
+    <t>//*[@id="id_gender2"]</t>
   </si>
 </sst>
 </file>
@@ -692,15 +707,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -740,590 +755,612 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="B35" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C35" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C36" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="3" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" t="s">
         <v>86</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>105</v>
+        <v>12</v>
+      </c>
+      <c r="C53" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C55" t="s">
-        <v>108</v>
+      <c r="C55" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B56">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B58">
       <formula1>"ID,ClassName,LinkText,CSS_Selector,TagName,Xpath,Name,PartialLinkText"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>